<commit_message>
Added product to inventory
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/TestDataA.xlsx
+++ b/src/main/java/com/testdata/TestDataA.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27004"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1889CB27-F0DF-4FC0-B07C-1461068CD696}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d8dbb31a7f2be120/Documents/Manual testcases/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="195" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7AA7005-6616-44A2-995A-D9CE4EBD7CDB}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Addproduct" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -22,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Username</t>
   </si>
@@ -52,13 +56,109 @@
   </si>
   <si>
     <t>@##$%</t>
+  </si>
+  <si>
+    <t>MS-01</t>
+  </si>
+  <si>
+    <t>SkWoods</t>
+  </si>
+  <si>
+    <t>teak-wood</t>
+  </si>
+  <si>
+    <t>illfordd</t>
+  </si>
+  <si>
+    <t>brown</t>
+  </si>
+  <si>
+    <t>SKDT</t>
+  </si>
+  <si>
+    <t>illfordd furniture</t>
+  </si>
+  <si>
+    <t>11A234GRS2</t>
+  </si>
+  <si>
+    <t>ModelNo</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>InvoiceNo</t>
+  </si>
+  <si>
+    <t>Podetails</t>
+  </si>
+  <si>
+    <t>RackName</t>
+  </si>
+  <si>
+    <t>HSNcode</t>
+  </si>
+  <si>
+    <t>Actual price</t>
+  </si>
+  <si>
+    <t>received data</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>breadth</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Item description</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Bedroom</t>
+  </si>
+  <si>
+    <t>InventoryStatus</t>
+  </si>
+  <si>
+    <t>To Be Sold</t>
+  </si>
+  <si>
+    <t>InventoryCondition</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>InventoryLocation</t>
+  </si>
+  <si>
+    <t>MRPFactor</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +173,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,7 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -105,6 +217,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -121,6 +241,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,17 +546,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -448,17 +572,17 @@
         <v>12345</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -466,7 +590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="35.25" customHeight="1">
+    <row r="6" spans="1:2" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1234567890</v>
       </c>
@@ -482,4 +606,194 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0644F360-2CCB-498F-B4D0-293D6C100F25}">
+  <dimension ref="A1:T16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="20.54296875" customWidth="1"/>
+    <col min="13" max="13" width="16.7265625" customWidth="1"/>
+    <col min="14" max="15" width="12.6328125" customWidth="1"/>
+    <col min="16" max="16" width="10.54296875" customWidth="1"/>
+    <col min="17" max="17" width="22.7265625" customWidth="1"/>
+    <col min="18" max="18" width="10.54296875" customWidth="1"/>
+    <col min="19" max="19" width="14.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4">
+        <v>182.9</v>
+      </c>
+      <c r="G2" s="4">
+        <v>35.6</v>
+      </c>
+      <c r="H2" s="4">
+        <v>61</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="5">
+        <v>45219</v>
+      </c>
+      <c r="N2" s="4">
+        <v>10000</v>
+      </c>
+      <c r="O2" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="P2" s="4">
+        <v>68132</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>